<commit_message>
qsub functions & more
</commit_message>
<xml_diff>
--- a/plume_settings.xlsx
+++ b/plume_settings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="48">
   <si>
     <t xml:space="preserve">C </t>
   </si>
@@ -134,6 +134,33 @@
   </si>
   <si>
     <t xml:space="preserve">Views 1 &amp; 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dn_32_2in_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi_dn32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dn_32_2in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi_dn32_rfun2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi_dn32_rfun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bi_dn32_rfun3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidn_32_2in_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidn_32_2in_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dn_32_rfun</t>
   </si>
   <si>
     <t xml:space="preserve">Views 3 &amp; 4</t>
@@ -213,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -262,6 +289,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -279,16 +314,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -409,7 +446,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="4" t="n">
-        <f aca="false">E5*B4</f>
+        <f aca="false">(E5*B4)</f>
         <v>0.072594</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -629,7 +666,9 @@
         <f aca="false">B1*B2*SQRT(B4)*(E11-B3*B5)^(2.5)</f>
         <v>0.00168114102220405</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="7" t="n">
+        <v>0.003</v>
+      </c>
       <c r="G14" s="5" t="s">
         <v>29</v>
       </c>
@@ -637,7 +676,9 @@
         <f aca="false">B1*B2*SQRT(B4)*(H11-B3*B5)^(2.5)</f>
         <v>0.00398313483035596</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="7" t="n">
+        <v>0.00898</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="11"/>
     </row>
@@ -657,7 +698,10 @@
         <f aca="false">1.225*3.1415*E12^2*E6</f>
         <v>0.000101382696922709</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5" t="n">
+        <f aca="false">1.225*3.1415*H12^2*E6</f>
+        <v>0.000101382696922709</v>
+      </c>
       <c r="G15" s="5" t="s">
         <v>31</v>
       </c>
@@ -665,7 +709,10 @@
         <f aca="false">1.225*3.1415*H12^2*E6</f>
         <v>0.000101382696922709</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="n">
+        <f aca="false">1.225*3.1415*H12^2*E6</f>
+        <v>0.000101382696922709</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
     </row>
@@ -680,7 +727,10 @@
         <f aca="false">E14/E15</f>
         <v>16.5821296259825</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5" t="n">
+        <f aca="false">F14/F15</f>
+        <v>29.5908482518187</v>
+      </c>
       <c r="G16" s="5" t="s">
         <v>28</v>
       </c>
@@ -688,7 +738,10 @@
         <f aca="false">H14/H15</f>
         <v>39.2881127771989</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="n">
+        <f aca="false">I14/I15</f>
+        <v>88.5752724337773</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
     </row>
@@ -701,9 +754,12 @@
       </c>
       <c r="E17" s="5" t="n">
         <f aca="false">E16*(1.225/B6)</f>
-        <v>0.00812524351673142</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>0.00812524351673141</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <f aca="false">F16*(1.225/B6)</f>
+        <v>0.0144995156433912</v>
+      </c>
       <c r="G17" s="5" t="s">
         <v>30</v>
       </c>
@@ -711,15 +767,16 @@
         <f aca="false">H16*(1.225/B6)</f>
         <v>0.0192511752608275</v>
       </c>
-      <c r="I17" s="5"/>
+      <c r="I17" s="5" t="n">
+        <f aca="false">I16*(1.225/B6)</f>
+        <v>0.0434018834925509</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="7" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="7" t="n">
@@ -730,7 +787,7 @@
       <c r="H18" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="I18" s="5"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
     </row>
@@ -1130,7 +1187,7 @@
       </c>
       <c r="D32" s="5" t="n">
         <f aca="false">D30/D31</f>
-        <v>9.76076322722429</v>
+        <v>9.76076322722428</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>26</v>
@@ -1212,25 +1269,50 @@
       <c r="J35" s="5"/>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="24.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="H36" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="J36" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="K36" s="6"/>
+      <c r="L36" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" s="5"/>
+      <c r="N36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O36" s="5"/>
+      <c r="P36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>0.0254</v>
+        <v>0.0508</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>35</v>
@@ -1250,13 +1332,43 @@
       <c r="H37" s="5" t="n">
         <v>0.0508</v>
       </c>
+      <c r="I37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="5" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L37" s="5" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37" s="5" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P37" s="5" t="n">
+        <v>0.0508</v>
+      </c>
+      <c r="Q37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R37" s="5" t="n">
+        <v>0.0508</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="7" t="n">
-        <v>0.00105</v>
+        <v>0.0027</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>15</v>
@@ -1273,7 +1385,39 @@
       <c r="G38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="7"/>
+      <c r="H38" s="7" t="n">
+        <v>9.4E-006</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="7" t="n">
+        <v>0.000171</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="7" t="n">
+        <v>2E-005</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="7" t="n">
+        <v>0.000827</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P38" s="7" t="n">
+        <v>0.00139</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R38" s="7" t="n">
+        <v>0.00259</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
@@ -1281,7 +1425,7 @@
       </c>
       <c r="B39" s="5" t="n">
         <f aca="false">1.225*B37^2*E6</f>
-        <v>5.7372562674E-005</v>
+        <v>0.000229490250696</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>26</v>
@@ -1304,6 +1448,41 @@
         <f aca="false">1.225*H37^2*E6</f>
         <v>0.000229490250696</v>
       </c>
+      <c r="I39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" s="5" t="n">
+        <f aca="false">1.225*J37^2*E6</f>
+        <v>0.000229490250696</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="5" t="n">
+        <f aca="false">1.225*L37^2*E6</f>
+        <v>0.000229490250696</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N39" s="5" t="n">
+        <f aca="false">1.225*N37^2*E6</f>
+        <v>0.000229490250696</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P39" s="5" t="n">
+        <f aca="false">1.225*P37^2*E6</f>
+        <v>0.000229490250696</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R39" s="5" t="n">
+        <f aca="false">1.225*R37^2*E6</f>
+        <v>0.000229490250696</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
@@ -1311,7 +1490,7 @@
       </c>
       <c r="B40" s="5" t="n">
         <f aca="false">B38/B39</f>
-        <v>18.3014310510455</v>
+        <v>11.7652056756721</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>28</v>
@@ -1332,7 +1511,42 @@
       </c>
       <c r="H40" s="5" t="n">
         <f aca="false">H38/H39</f>
-        <v>0</v>
+        <v>0.0409603456856733</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="5" t="n">
+        <f aca="false">J38/J39</f>
+        <v>0.745129692792568</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L40" s="5" t="n">
+        <f aca="false">L38/L39</f>
+        <v>0.0871496716716454</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="5" t="n">
+        <f aca="false">N38/N39</f>
+        <v>3.60363892362254</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P40" s="5" t="n">
+        <f aca="false">P38/P39</f>
+        <v>6.05690218117936</v>
+      </c>
+      <c r="Q40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R40" s="5" t="n">
+        <f aca="false">R38/R39</f>
+        <v>11.2858824814781</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,7 +1555,7 @@
       </c>
       <c r="B41" s="5" t="n">
         <f aca="false">B40*1.225/B6</f>
-        <v>0.00896770121501232</v>
+        <v>0.00576495078107935</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>30</v>
@@ -1362,7 +1576,42 @@
       </c>
       <c r="H41" s="5" t="n">
         <f aca="false">H40*1.225/2500</f>
-        <v>0</v>
+        <v>2.00705693859799E-005</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J41" s="5" t="n">
+        <f aca="false">J40*1.225/2500</f>
+        <v>0.000365113549468358</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="5" t="n">
+        <f aca="false">L40*1.225/2500</f>
+        <v>4.27033391191063E-005</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" s="5" t="n">
+        <f aca="false">N40*1.225/B6</f>
+        <v>0.00176578307257504</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P41" s="5" t="n">
+        <f aca="false">P40*1.225/B6</f>
+        <v>0.00296788206877788</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R41" s="5" t="n">
+        <f aca="false">R40*1.225/B6</f>
+        <v>0.00553008241592426</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1652,9 @@
         <v>0.00053</v>
       </c>
       <c r="E44" s="5"/>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7" t="n">
+        <v>0.00022949</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
@@ -1411,7 +1662,7 @@
       </c>
       <c r="B45" s="5" t="n">
         <f aca="false">1.225*B37^2*E6</f>
-        <v>5.7372562674E-005</v>
+        <v>0.000229490250696</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>26</v>
@@ -1429,7 +1680,7 @@
       </c>
       <c r="B46" s="5" t="n">
         <f aca="false">B44/B45</f>
-        <v>18.4757303943888</v>
+        <v>4.61893259859721</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>28</v>
@@ -1447,7 +1698,7 @@
       </c>
       <c r="B47" s="5" t="n">
         <f aca="false">B46*1.225/2500</f>
-        <v>0.00905310789325053</v>
+        <v>0.00226327697331263</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>30</v>
@@ -1465,16 +1716,224 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5"/>
+    <row r="51" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="13"/>
+      <c r="G70" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K72" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K73" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>